<commit_message>
Se agregaron longitudes y latitudes al archivo de localidades
</commit_message>
<xml_diff>
--- a/Mapa/localidades.xlsx
+++ b/Mapa/localidades.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/if714983_iteso_mx/Documents/ITESO/8avo semestre/PAP/ExelPitss_Equipo4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria jose\Documents\ITESO\ExelPitss\Mapa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{3575B968-361F-4493-9A7B-EC04DE7F3813}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{079E3307-0A45-45DA-B7E3-EA816F204083}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F8CC178E-864D-4A6D-A1A7-0BEBD841B630}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -381,7 +380,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,14 +430,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DC86063-4E70-45A3-957E-6DBA2743B297}" name="Tabla1" displayName="Tabla1" ref="A1:B83" totalsRowShown="0">
-  <autoFilter ref="A1:B83" xr:uid="{EE4183D9-753B-4CB0-A126-6C97BAEC197D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B83">
-    <sortCondition ref="A1:A83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B83" totalsRowShown="0">
+  <autoFilter ref="A1:B83"/>
+  <sortState ref="A2:D83">
+    <sortCondition ref="B1:B83"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7938AA94-4EC6-4D94-A1B2-3A13F767D07F}" name="APELLIDOS Y NOMBRES"/>
-    <tableColumn id="2" xr3:uid="{D2E1783F-C1A6-42D1-9D88-88484308EA27}" name="Zona"/>
+    <tableColumn id="1" name="APELLIDOS Y NOMBRES"/>
+    <tableColumn id="2" name="Zona"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -740,20 +739,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115F259F-7C2B-4297-9091-583CEE8EE219}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -761,399 +760,399 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>6</v>
       </c>
-      <c r="B27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="B29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="B32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
-      <c r="B34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>0</v>
       </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>111</v>
-      </c>
       <c r="B43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1161,260 +1160,260 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
+      <c r="B75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>56</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B80" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>39</v>
-      </c>
-      <c r="B62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>16</v>
-      </c>
-      <c r="B65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>27</v>
-      </c>
-      <c r="B66" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>43</v>
-      </c>
-      <c r="B68" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>49</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B81" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>34</v>
-      </c>
-      <c r="B76" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>47</v>
-      </c>
-      <c r="B77" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>45</v>
-      </c>
-      <c r="B79" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>78</v>
-      </c>
-      <c r="B81" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>